<commit_message>
add ip asn download
</commit_message>
<xml_diff>
--- a/ipasn.xlsx
+++ b/ipasn.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S104"/>
+  <dimension ref="A1:W104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,21 +443,33 @@
         <v>ipasn_kualifikasi</v>
       </c>
       <c r="N1" t="str">
+        <v>ip_asn_keterangan_kualifikasi</v>
+      </c>
+      <c r="O1" t="str">
         <v>ipasn_kompetensi</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
+        <v>ip_asn_keterangan_kompetensi</v>
+      </c>
+      <c r="Q1" t="str">
         <v>ipasn_kinerja</v>
       </c>
-      <c r="P1" t="str">
+      <c r="R1" t="str">
+        <v>ip_asn_keterangan_kinerja</v>
+      </c>
+      <c r="S1" t="str">
         <v>ipasn_disiplin</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="T1" t="str">
+        <v>ip_asn_keterangan_disiplin</v>
+      </c>
+      <c r="U1" t="str">
         <v>ipasn_total</v>
       </c>
-      <c r="R1" t="str">
+      <c r="V1" t="str">
         <v>ipasn_tahun</v>
       </c>
-      <c r="S1" t="str">
+      <c r="W1" t="str">
         <v>ipasn_updated</v>
       </c>
     </row>
@@ -499,7 +511,7 @@
         <v>PNS</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" xml:space="preserve">
       <c r="A3">
         <v>2</v>
       </c>
@@ -540,25 +552,39 @@
         <v>23.00</v>
       </c>
       <c r="N3" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O3" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="P3" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q3" t="str">
         <v>30.00</v>
       </c>
-      <c r="P3" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q3" t="str">
-        <v>68.00</v>
-      </c>
-      <c r="R3">
-        <v>2023</v>
+      <c r="R3" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S3" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>5.00</v>
+      </c>
+      <c r="T3" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U3" t="str">
+        <v>83.00</v>
+      </c>
+      <c r="V3">
+        <v>2023</v>
+      </c>
+      <c r="W3" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
       <c r="A4">
         <v>3</v>
       </c>
@@ -596,25 +622,39 @@
         <v>20.00</v>
       </c>
       <c r="N4" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA Kejuruan</v>
       </c>
       <c r="O4" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P4" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q4" t="str">
         <v>25.00</v>
       </c>
-      <c r="P4" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q4" t="str">
-        <v>67.50</v>
-      </c>
-      <c r="R4">
-        <v>2023</v>
+      <c r="R4" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S4" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>5.00</v>
+      </c>
+      <c r="T4" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U4" t="str">
+        <v>90.00</v>
+      </c>
+      <c r="V4">
+        <v>2023</v>
+      </c>
+      <c r="W4" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
       <c r="A5">
         <v>4</v>
       </c>
@@ -655,25 +695,39 @@
         <v>21.00</v>
       </c>
       <c r="N5" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma III/Sarjana Muda</v>
       </c>
       <c r="O5" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P5" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q5" t="str">
         <v>30.00</v>
       </c>
-      <c r="P5" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q5" t="str">
-        <v>73.50</v>
-      </c>
-      <c r="R5">
-        <v>2023</v>
+      <c r="R5" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S5" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5.00</v>
+      </c>
+      <c r="T5" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U5" t="str">
+        <v>96.00</v>
+      </c>
+      <c r="V5">
+        <v>2023</v>
+      </c>
+      <c r="W5" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
       <c r="A6">
         <v>5</v>
       </c>
@@ -714,25 +768,39 @@
         <v>23.00</v>
       </c>
       <c r="N6" t="str">
-        <v>15.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O6" t="str">
         <v>30.00</v>
       </c>
-      <c r="P6" t="str">
-        <v>5.00</v>
+      <c r="P6" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda belum sama sekali melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q6" t="str">
-        <v>73.00</v>
-      </c>
-      <c r="R6">
-        <v>2023</v>
+        <v>30.00</v>
+      </c>
+      <c r="R6" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S6" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>5.00</v>
+      </c>
+      <c r="T6" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U6" t="str">
+        <v>88.00</v>
+      </c>
+      <c r="V6">
+        <v>2023</v>
+      </c>
+      <c r="W6" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
       <c r="A7">
         <v>6</v>
       </c>
@@ -773,25 +841,39 @@
         <v>22.00</v>
       </c>
       <c r="N7" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O7" t="str">
         <v>40.00</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q7" t="str">
         <v>25.00</v>
       </c>
-      <c r="P7" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q7" t="str">
+      <c r="R7" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S7" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T7" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U7" t="str">
         <v>92.00</v>
       </c>
-      <c r="R7">
-        <v>2023</v>
-      </c>
-      <c r="S7" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="V7">
+        <v>2023</v>
+      </c>
+      <c r="W7" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
       <c r="A8">
         <v>7</v>
       </c>
@@ -832,25 +914,39 @@
         <v>23.00</v>
       </c>
       <c r="N8" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O8" t="str">
         <v>40.00</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P8" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 122 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q8" t="str">
         <v>30.00</v>
       </c>
-      <c r="P8" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S8" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T8" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U8" t="str">
         <v>98.00</v>
       </c>
-      <c r="R8">
-        <v>2023</v>
-      </c>
-      <c r="S8" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="V8">
+        <v>2023</v>
+      </c>
+      <c r="W8" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="9" xml:space="preserve">
       <c r="A9">
         <v>8</v>
       </c>
@@ -891,25 +987,39 @@
         <v>20.00</v>
       </c>
       <c r="N9" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O9" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P9" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q9" t="str">
         <v>30.00</v>
       </c>
-      <c r="P9" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q9" t="str">
-        <v>80.00</v>
-      </c>
-      <c r="R9">
-        <v>2023</v>
+      <c r="R9" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S9" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>5.00</v>
+      </c>
+      <c r="T9" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U9" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V9">
+        <v>2023</v>
+      </c>
+      <c r="W9" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
       <c r="A10">
         <v>9</v>
       </c>
@@ -950,25 +1060,39 @@
         <v>23.00</v>
       </c>
       <c r="N10" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O10" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P10" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q10" t="str">
         <v>30.00</v>
       </c>
-      <c r="P10" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>83.00</v>
-      </c>
-      <c r="R10">
-        <v>2023</v>
+      <c r="R10" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S10" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>5.00</v>
+      </c>
+      <c r="T10" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U10" t="str">
+        <v>98.00</v>
+      </c>
+      <c r="V10">
+        <v>2023</v>
+      </c>
+      <c r="W10" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="11" xml:space="preserve">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1009,25 +1133,39 @@
         <v>23.00</v>
       </c>
       <c r="N11" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O11" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P11" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q11" t="str">
         <v>30.00</v>
       </c>
-      <c r="P11" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q11" t="str">
-        <v>83.00</v>
-      </c>
-      <c r="R11">
-        <v>2023</v>
+      <c r="R11" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S11" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>5.00</v>
+      </c>
+      <c r="T11" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U11" t="str">
+        <v>98.00</v>
+      </c>
+      <c r="V11">
+        <v>2023</v>
+      </c>
+      <c r="W11" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="12" xml:space="preserve">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1068,25 +1206,39 @@
         <v>23.00</v>
       </c>
       <c r="N12" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O12" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P12" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 46 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q12" t="str">
         <v>25.00</v>
       </c>
-      <c r="O12" t="str">
-        <v>25.00</v>
-      </c>
-      <c r="P12" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q12" t="str">
-        <v>78.00</v>
-      </c>
-      <c r="R12">
-        <v>2023</v>
+      <c r="R12" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S12" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>5.00</v>
+      </c>
+      <c r="T12" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U12" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V12">
+        <v>2023</v>
+      </c>
+      <c r="W12" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="13" xml:space="preserve">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1127,25 +1279,39 @@
         <v>23.00</v>
       </c>
       <c r="N13" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O13" t="str">
         <v>25.00</v>
       </c>
-      <c r="P13" t="str">
-        <v>5.00</v>
+      <c r="P13" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q13" t="str">
-        <v>63.00</v>
-      </c>
-      <c r="R13">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R13" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S13" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>5.00</v>
+      </c>
+      <c r="T13" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U13" t="str">
+        <v>78.00</v>
+      </c>
+      <c r="V13">
+        <v>2023</v>
+      </c>
+      <c r="W13" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="14" xml:space="preserve">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1186,25 +1352,39 @@
         <v>20.00</v>
       </c>
       <c r="N14" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O14" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P14" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q14" t="str">
         <v>30.00</v>
       </c>
-      <c r="P14" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q14" t="str">
-        <v>80.00</v>
-      </c>
-      <c r="R14">
-        <v>2023</v>
+      <c r="R14" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S14" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>5.00</v>
+      </c>
+      <c r="T14" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U14" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V14">
+        <v>2023</v>
+      </c>
+      <c r="W14" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="15" xml:space="preserve">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1245,25 +1425,39 @@
         <v>23.00</v>
       </c>
       <c r="N15" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O15" t="str">
         <v>17.50</v>
       </c>
-      <c r="O15" t="str">
+      <c r="P15" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q15" t="str">
         <v>25.00</v>
       </c>
-      <c r="P15" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q15" t="str">
+      <c r="R15" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S15" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T15" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U15" t="str">
         <v>70.50</v>
       </c>
-      <c r="R15">
-        <v>2023</v>
-      </c>
-      <c r="S15" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="V15">
+        <v>2023</v>
+      </c>
+      <c r="W15" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="16" xml:space="preserve">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1298,25 +1492,39 @@
         <v>22.00</v>
       </c>
       <c r="N16" t="str">
-        <v>0.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O16" t="str">
         <v>0.00</v>
       </c>
-      <c r="P16" t="str">
-        <v>5.00</v>
+      <c r="P16" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda belum sama sekali melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q16" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="R16" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, ''</v>
+      </c>
+      <c r="S16" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T16" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U16" t="str">
         <v>27.00</v>
       </c>
-      <c r="R16">
-        <v>2023</v>
-      </c>
-      <c r="S16" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="V16">
+        <v>2023</v>
+      </c>
+      <c r="W16" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="17" xml:space="preserve">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1342,10 +1550,10 @@
         <v>ILMU SOSIAL</v>
       </c>
       <c r="I17" t="str">
-        <v>III/c</v>
+        <v>III/d</v>
       </c>
       <c r="J17" t="str">
-        <v>Penata</v>
+        <v>Penata Tingkat I</v>
       </c>
       <c r="K17" t="str">
         <v>Analis Sumber Daya Manusia Aparatur Ahli Muda (III/c)</v>
@@ -1357,25 +1565,39 @@
         <v>23.00</v>
       </c>
       <c r="N17" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O17" t="str">
         <v>40.00</v>
       </c>
-      <c r="O17" t="str">
+      <c r="P17" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 70 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q17" t="str">
         <v>30.00</v>
       </c>
-      <c r="P17" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q17" t="str">
+      <c r="R17" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S17" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T17" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U17" t="str">
         <v>98.00</v>
       </c>
-      <c r="R17">
-        <v>2023</v>
-      </c>
-      <c r="S17" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="V17">
+        <v>2023</v>
+      </c>
+      <c r="W17" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="18" xml:space="preserve">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1416,25 +1638,39 @@
         <v>20.00</v>
       </c>
       <c r="N18" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O18" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P18" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q18" t="str">
         <v>30.00</v>
       </c>
-      <c r="P18" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q18" t="str">
-        <v>80.00</v>
-      </c>
-      <c r="R18">
-        <v>2023</v>
+      <c r="R18" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S18" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>5.00</v>
+      </c>
+      <c r="T18" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U18" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V18">
+        <v>2023</v>
+      </c>
+      <c r="W18" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="19" xml:space="preserve">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1475,25 +1711,39 @@
         <v>23.00</v>
       </c>
       <c r="N19" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O19" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P19" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q19" t="str">
         <v>25.00</v>
       </c>
-      <c r="P19" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q19" t="str">
-        <v>70.50</v>
-      </c>
-      <c r="R19">
-        <v>2023</v>
+      <c r="R19" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S19" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>5.00</v>
+      </c>
+      <c r="T19" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U19" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V19">
+        <v>2023</v>
+      </c>
+      <c r="W19" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="20" xml:space="preserve">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1534,25 +1784,39 @@
         <v>22.00</v>
       </c>
       <c r="N20" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O20" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P20" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q20" t="str">
         <v>25.00</v>
       </c>
-      <c r="P20" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q20" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R20">
-        <v>2023</v>
+      <c r="R20" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S20" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>5.00</v>
+      </c>
+      <c r="T20" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U20" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V20">
+        <v>2023</v>
+      </c>
+      <c r="W20" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="21" xml:space="preserve">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1593,25 +1857,39 @@
         <v>23.00</v>
       </c>
       <c r="N21" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O21" t="str">
         <v>25.00</v>
       </c>
-      <c r="P21" t="str">
-        <v>5.00</v>
+      <c r="P21" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q21" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="R21" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S21" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T21" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U21" t="str">
         <v>78.00</v>
       </c>
-      <c r="R21">
-        <v>2023</v>
-      </c>
-      <c r="S21" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="22">
+      <c r="V21">
+        <v>2023</v>
+      </c>
+      <c r="W21" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="22" xml:space="preserve">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1652,25 +1930,39 @@
         <v>22.00</v>
       </c>
       <c r="N22" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O22" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P22" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q22" t="str">
         <v>30.00</v>
       </c>
-      <c r="P22" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q22" t="str">
-        <v>74.50</v>
-      </c>
-      <c r="R22">
-        <v>2023</v>
+      <c r="R22" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S22" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>5.00</v>
+      </c>
+      <c r="T22" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U22" t="str">
+        <v>97.00</v>
+      </c>
+      <c r="V22">
+        <v>2023</v>
+      </c>
+      <c r="W22" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="23" xml:space="preserve">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1711,25 +2003,39 @@
         <v>23.00</v>
       </c>
       <c r="N23" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O23" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P23" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q23" t="str">
         <v>25.00</v>
       </c>
-      <c r="P23" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q23" t="str">
-        <v>70.50</v>
-      </c>
-      <c r="R23">
-        <v>2023</v>
+      <c r="R23" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S23" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>5.00</v>
+      </c>
+      <c r="T23" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U23" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V23">
+        <v>2023</v>
+      </c>
+      <c r="W23" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="24" xml:space="preserve">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1770,25 +2076,39 @@
         <v>20.00</v>
       </c>
       <c r="N24" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O24" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P24" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q24" t="str">
         <v>30.00</v>
       </c>
-      <c r="P24" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q24" t="str">
-        <v>80.00</v>
-      </c>
-      <c r="R24">
-        <v>2023</v>
+      <c r="R24" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S24" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>5.00</v>
+      </c>
+      <c r="T24" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U24" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V24">
+        <v>2023</v>
+      </c>
+      <c r="W24" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="25" xml:space="preserve">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1829,22 +2149,36 @@
         <v>20.00</v>
       </c>
       <c r="N25" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O25" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P25" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q25" t="str">
         <v>30.00</v>
       </c>
-      <c r="P25" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q25" t="str">
-        <v>80.00</v>
-      </c>
-      <c r="R25">
-        <v>2023</v>
+      <c r="R25" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S25" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T25" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U25" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V25">
+        <v>2023</v>
+      </c>
+      <c r="W25" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="26">
@@ -1885,7 +2219,7 @@
         <v>PPPK</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" xml:space="preserve">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1926,25 +2260,39 @@
         <v>20.00</v>
       </c>
       <c r="N27" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O27" t="str">
         <v>25.00</v>
       </c>
-      <c r="O27" t="str">
+      <c r="P27" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q27" t="str">
         <v>30.00</v>
       </c>
-      <c r="P27" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q27" t="str">
+      <c r="R27" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S27" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T27" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U27" t="str">
         <v>80.00</v>
       </c>
-      <c r="R27">
-        <v>2023</v>
-      </c>
-      <c r="S27" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="28">
+      <c r="V27">
+        <v>2023</v>
+      </c>
+      <c r="W27" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="28" xml:space="preserve">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1985,22 +2333,36 @@
         <v>20.00</v>
       </c>
       <c r="N28" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O28" t="str">
         <v>25.00</v>
       </c>
-      <c r="O28" t="str">
+      <c r="P28" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q28" t="str">
         <v>30.00</v>
       </c>
-      <c r="P28" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q28" t="str">
+      <c r="R28" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S28" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T28" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U28" t="str">
         <v>80.00</v>
       </c>
-      <c r="R28">
-        <v>2023</v>
-      </c>
-      <c r="S28" t="str">
-        <v>8-March-2024</v>
+      <c r="V28">
+        <v>2023</v>
+      </c>
+      <c r="W28" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="29">
@@ -2040,29 +2402,8 @@
       <c r="L29" t="str">
         <v>PNS</v>
       </c>
-      <c r="M29" t="str">
-        <v>22.00</v>
-      </c>
-      <c r="N29" t="str">
-        <v>17.50</v>
-      </c>
-      <c r="O29" t="str">
-        <v>25.00</v>
-      </c>
-      <c r="P29" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q29" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R29">
-        <v>2023</v>
-      </c>
-      <c r="S29" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="30">
+    </row>
+    <row r="30" xml:space="preserve">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2103,25 +2444,39 @@
         <v>23.00</v>
       </c>
       <c r="N30" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O30" t="str">
         <v>10.00</v>
       </c>
-      <c r="O30" t="str">
+      <c r="P30" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q30" t="str">
         <v>25.00</v>
       </c>
-      <c r="P30" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q30" t="str">
+      <c r="R30" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S30" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T30" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U30" t="str">
         <v>63.00</v>
       </c>
-      <c r="R30">
-        <v>2023</v>
-      </c>
-      <c r="S30" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="V30">
+        <v>2023</v>
+      </c>
+      <c r="W30" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="31" xml:space="preserve">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2162,25 +2517,39 @@
         <v>20.00</v>
       </c>
       <c r="N31" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O31" t="str">
         <v>40.00</v>
       </c>
-      <c r="O31" t="str">
+      <c r="P31" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q31" t="str">
         <v>30.00</v>
       </c>
-      <c r="P31" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q31" t="str">
+      <c r="R31" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S31" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T31" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U31" t="str">
         <v>95.00</v>
       </c>
-      <c r="R31">
-        <v>2023</v>
-      </c>
-      <c r="S31" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="32">
+      <c r="V31">
+        <v>2023</v>
+      </c>
+      <c r="W31" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="32" xml:space="preserve">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2221,25 +2590,39 @@
         <v>22.00</v>
       </c>
       <c r="N32" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O32" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P32" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q32" t="str">
         <v>25.00</v>
       </c>
-      <c r="P32" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q32" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R32">
-        <v>2023</v>
+      <c r="R32" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S32" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>5.00</v>
+      </c>
+      <c r="T32" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U32" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V32">
+        <v>2023</v>
+      </c>
+      <c r="W32" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="33" xml:space="preserve">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2280,22 +2663,36 @@
         <v>23.00</v>
       </c>
       <c r="N33" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O33" t="str">
         <v>40.00</v>
       </c>
-      <c r="O33" t="str">
+      <c r="P33" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q33" t="str">
         <v>25.00</v>
       </c>
-      <c r="P33" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q33" t="str">
+      <c r="R33" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S33" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T33" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U33" t="str">
         <v>93.00</v>
       </c>
-      <c r="R33">
-        <v>2023</v>
-      </c>
-      <c r="S33" t="str">
-        <v>8-March-2024</v>
+      <c r="V33">
+        <v>2023</v>
+      </c>
+      <c r="W33" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="34">
@@ -2336,7 +2733,7 @@
         <v>PPPK</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" xml:space="preserve">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2377,25 +2774,39 @@
         <v>23.00</v>
       </c>
       <c r="N35" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O35" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P35" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 54 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q35" t="str">
         <v>25.00</v>
       </c>
-      <c r="P35" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q35" t="str">
-        <v>70.50</v>
-      </c>
-      <c r="R35">
-        <v>2023</v>
+      <c r="R35" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S35" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>5.00</v>
+      </c>
+      <c r="T35" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U35" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V35">
+        <v>2023</v>
+      </c>
+      <c r="W35" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="36" xml:space="preserve">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2436,25 +2847,39 @@
         <v>22.00</v>
       </c>
       <c r="N36" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma III/Sarjana Muda</v>
       </c>
       <c r="O36" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P36" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q36" t="str">
         <v>25.00</v>
       </c>
-      <c r="P36" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q36" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R36">
-        <v>2023</v>
+      <c r="R36" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S36" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>5.00</v>
+      </c>
+      <c r="T36" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U36" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V36">
+        <v>2023</v>
+      </c>
+      <c r="W36" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="37" xml:space="preserve">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2495,25 +2920,39 @@
         <v>23.00</v>
       </c>
       <c r="N37" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O37" t="str">
         <v>40.00</v>
       </c>
-      <c r="O37" t="str">
+      <c r="P37" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 55 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q37" t="str">
         <v>30.00</v>
       </c>
-      <c r="P37" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q37" t="str">
+      <c r="R37" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S37" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T37" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U37" t="str">
         <v>98.00</v>
       </c>
-      <c r="R37">
-        <v>2023</v>
-      </c>
-      <c r="S37" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="38">
+      <c r="V37">
+        <v>2023</v>
+      </c>
+      <c r="W37" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="38" xml:space="preserve">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2554,25 +2993,39 @@
         <v>23.00</v>
       </c>
       <c r="N38" t="str">
-        <v>30.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O38" t="str">
         <v>30.00</v>
       </c>
-      <c r="P38" t="str">
-        <v>5.00</v>
+      <c r="P38" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 66 Jam_x000d_
+Anda belum sama sekali melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q38" t="str">
+        <v>30.00</v>
+      </c>
+      <c r="R38" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S38" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T38" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U38" t="str">
         <v>88.00</v>
       </c>
-      <c r="R38">
-        <v>2023</v>
-      </c>
-      <c r="S38" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="39">
+      <c r="V38">
+        <v>2023</v>
+      </c>
+      <c r="W38" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="39" xml:space="preserve">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2613,22 +3066,36 @@
         <v>22.00</v>
       </c>
       <c r="N39" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O39" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P39" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q39" t="str">
         <v>25.00</v>
       </c>
-      <c r="P39" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q39" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R39">
-        <v>2023</v>
+      <c r="R39" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S39" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T39" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U39" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V39">
+        <v>2023</v>
+      </c>
+      <c r="W39" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="40">
@@ -2669,7 +3136,7 @@
         <v>PPPK</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" xml:space="preserve">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2710,22 +3177,36 @@
         <v>22.00</v>
       </c>
       <c r="N41" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O41" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P41" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q41" t="str">
         <v>25.00</v>
       </c>
-      <c r="P41" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q41" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R41">
-        <v>2023</v>
+      <c r="R41" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S41" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T41" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U41" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V41">
+        <v>2023</v>
+      </c>
+      <c r="W41" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="42">
@@ -2766,7 +3247,7 @@
         <v>PNS</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" xml:space="preserve">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2807,25 +3288,39 @@
         <v>23.00</v>
       </c>
       <c r="N43" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O43" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P43" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q43" t="str">
         <v>25.00</v>
       </c>
-      <c r="O43" t="str">
-        <v>25.00</v>
-      </c>
-      <c r="P43" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q43" t="str">
-        <v>78.00</v>
-      </c>
-      <c r="R43">
-        <v>2023</v>
+      <c r="R43" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S43" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>5.00</v>
+      </c>
+      <c r="T43" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U43" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V43">
+        <v>2023</v>
+      </c>
+      <c r="W43" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="44" xml:space="preserve">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2866,25 +3361,39 @@
         <v>22.00</v>
       </c>
       <c r="N44" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O44" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P44" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q44" t="str">
         <v>25.00</v>
       </c>
-      <c r="P44" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q44" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R44">
-        <v>2023</v>
+      <c r="R44" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S44" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>5.00</v>
+      </c>
+      <c r="T44" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U44" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V44">
+        <v>2023</v>
+      </c>
+      <c r="W44" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="45" xml:space="preserve">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2925,22 +3434,36 @@
         <v>21.00</v>
       </c>
       <c r="N45" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O45" t="str">
         <v>25.00</v>
       </c>
-      <c r="P45" t="str">
-        <v>5.00</v>
+      <c r="P45" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q45" t="str">
-        <v>61.00</v>
-      </c>
-      <c r="R45">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R45" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S45" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T45" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U45" t="str">
+        <v>76.00</v>
+      </c>
+      <c r="V45">
+        <v>2023</v>
+      </c>
+      <c r="W45" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="46">
@@ -2981,7 +3504,7 @@
         <v>PNS</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" xml:space="preserve">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3022,25 +3545,39 @@
         <v>20.00</v>
       </c>
       <c r="N47" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O47" t="str">
         <v>25.00</v>
       </c>
-      <c r="O47" t="str">
+      <c r="P47" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q47" t="str">
         <v>30.00</v>
       </c>
-      <c r="P47" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q47" t="str">
+      <c r="R47" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S47" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T47" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U47" t="str">
         <v>80.00</v>
       </c>
-      <c r="R47">
-        <v>2023</v>
-      </c>
-      <c r="S47" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="48">
+      <c r="V47">
+        <v>2023</v>
+      </c>
+      <c r="W47" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="48" xml:space="preserve">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3081,22 +3618,36 @@
         <v>23.00</v>
       </c>
       <c r="N48" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O48" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P48" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 98 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q48" t="str">
         <v>30.00</v>
       </c>
-      <c r="P48" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q48" t="str">
-        <v>83.00</v>
-      </c>
-      <c r="R48">
-        <v>2023</v>
+      <c r="R48" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S48" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T48" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U48" t="str">
+        <v>98.00</v>
+      </c>
+      <c r="V48">
+        <v>2023</v>
+      </c>
+      <c r="W48" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="49">
@@ -3137,7 +3688,7 @@
         <v>PPPK</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" xml:space="preserve">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3175,25 +3726,39 @@
         <v>20.00</v>
       </c>
       <c r="N50" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA Kejuruan</v>
       </c>
       <c r="O50" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P50" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q50" t="str">
         <v>25.00</v>
       </c>
-      <c r="P50" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q50" t="str">
-        <v>67.50</v>
-      </c>
-      <c r="R50">
-        <v>2023</v>
+      <c r="R50" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S50" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>5.00</v>
+      </c>
+      <c r="T50" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U50" t="str">
+        <v>90.00</v>
+      </c>
+      <c r="V50">
+        <v>2023</v>
+      </c>
+      <c r="W50" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="51" xml:space="preserve">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3234,25 +3799,39 @@
         <v>23.00</v>
       </c>
       <c r="N51" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
+      </c>
+      <c r="O51" t="str">
         <v>40.00</v>
       </c>
-      <c r="O51" t="str">
+      <c r="P51" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q51" t="str">
         <v>25.00</v>
       </c>
-      <c r="P51" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q51" t="str">
+      <c r="R51" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S51" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T51" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U51" t="str">
         <v>93.00</v>
       </c>
-      <c r="R51">
-        <v>2023</v>
-      </c>
-      <c r="S51" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="52">
+      <c r="V51">
+        <v>2023</v>
+      </c>
+      <c r="W51" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="52" xml:space="preserve">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3293,25 +3872,39 @@
         <v>20.00</v>
       </c>
       <c r="N52" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O52" t="str">
         <v>40.00</v>
       </c>
-      <c r="O52" t="str">
+      <c r="P52" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q52" t="str">
         <v>25.00</v>
       </c>
-      <c r="P52" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q52" t="str">
+      <c r="R52" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S52" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T52" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U52" t="str">
         <v>90.00</v>
       </c>
-      <c r="R52">
-        <v>2023</v>
-      </c>
-      <c r="S52" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="53">
+      <c r="V52">
+        <v>2023</v>
+      </c>
+      <c r="W52" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="53" xml:space="preserve">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3352,25 +3945,39 @@
         <v>20.00</v>
       </c>
       <c r="N53" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O53" t="str">
         <v>40.00</v>
       </c>
-      <c r="O53" t="str">
+      <c r="P53" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q53" t="str">
         <v>25.00</v>
       </c>
-      <c r="P53" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q53" t="str">
+      <c r="R53" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S53" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T53" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U53" t="str">
         <v>90.00</v>
       </c>
-      <c r="R53">
-        <v>2023</v>
-      </c>
-      <c r="S53" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="54">
+      <c r="V53">
+        <v>2023</v>
+      </c>
+      <c r="W53" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="54" xml:space="preserve">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3411,22 +4018,36 @@
         <v>23.00</v>
       </c>
       <c r="N54" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O54" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P54" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 20 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q54" t="str">
         <v>25.00</v>
       </c>
-      <c r="P54" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q54" t="str">
-        <v>70.50</v>
-      </c>
-      <c r="R54">
-        <v>2023</v>
+      <c r="R54" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S54" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T54" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U54" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V54">
+        <v>2023</v>
+      </c>
+      <c r="W54" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="55">
@@ -3466,29 +4087,8 @@
       <c r="L55" t="str">
         <v>PNS</v>
       </c>
-      <c r="M55" t="str">
-        <v>22.00</v>
-      </c>
-      <c r="N55" t="str">
-        <v>17.50</v>
-      </c>
-      <c r="O55" t="str">
-        <v>25.00</v>
-      </c>
-      <c r="P55" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q55" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R55">
-        <v>2023</v>
-      </c>
-      <c r="S55" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="56">
+    </row>
+    <row r="56" xml:space="preserve">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3529,22 +4129,36 @@
         <v>22.00</v>
       </c>
       <c r="N56" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O56" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P56" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q56" t="str">
         <v>30.00</v>
       </c>
-      <c r="P56" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q56" t="str">
-        <v>74.50</v>
-      </c>
-      <c r="R56">
-        <v>2023</v>
+      <c r="R56" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S56" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T56" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U56" t="str">
+        <v>97.00</v>
+      </c>
+      <c r="V56">
+        <v>2023</v>
+      </c>
+      <c r="W56" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="57">
@@ -3585,7 +4199,7 @@
         <v>PPPK</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" xml:space="preserve">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3626,25 +4240,39 @@
         <v>21.00</v>
       </c>
       <c r="N58" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O58" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="P58" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q58" t="str">
         <v>30.00</v>
       </c>
-      <c r="P58" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q58" t="str">
-        <v>66.00</v>
-      </c>
-      <c r="R58">
-        <v>2023</v>
+      <c r="R58" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S58" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>5.00</v>
+      </c>
+      <c r="T58" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U58" t="str">
+        <v>81.00</v>
+      </c>
+      <c r="V58">
+        <v>2023</v>
+      </c>
+      <c r="W58" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="59" xml:space="preserve">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3685,25 +4313,39 @@
         <v>22.00</v>
       </c>
       <c r="N59" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O59" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P59" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q59" t="str">
         <v>25.00</v>
       </c>
-      <c r="P59" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q59" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R59">
-        <v>2023</v>
+      <c r="R59" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S59" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>5.00</v>
+      </c>
+      <c r="T59" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U59" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V59">
+        <v>2023</v>
+      </c>
+      <c r="W59" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="60" xml:space="preserve">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3744,25 +4386,39 @@
         <v>20.00</v>
       </c>
       <c r="N60" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O60" t="str">
         <v>40.00</v>
       </c>
-      <c r="O60" t="str">
+      <c r="P60" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q60" t="str">
         <v>30.00</v>
       </c>
-      <c r="P60" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q60" t="str">
+      <c r="R60" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S60" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T60" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U60" t="str">
         <v>95.00</v>
       </c>
-      <c r="R60">
-        <v>2023</v>
-      </c>
-      <c r="S60" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="61">
+      <c r="V60">
+        <v>2023</v>
+      </c>
+      <c r="W60" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="61" xml:space="preserve">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3800,25 +4456,39 @@
         <v>20.00</v>
       </c>
       <c r="N61" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA</v>
       </c>
       <c r="O61" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P61" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q61" t="str">
         <v>25.00</v>
       </c>
-      <c r="P61" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q61" t="str">
-        <v>67.50</v>
-      </c>
-      <c r="R61">
-        <v>2023</v>
+      <c r="R61" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S61" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>5.00</v>
+      </c>
+      <c r="T61" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U61" t="str">
+        <v>90.00</v>
+      </c>
+      <c r="V61">
+        <v>2023</v>
+      </c>
+      <c r="W61" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="62" xml:space="preserve">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3859,25 +4529,39 @@
         <v>23.00</v>
       </c>
       <c r="N62" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O62" t="str">
         <v>25.00</v>
       </c>
-      <c r="P62" t="str">
-        <v>5.00</v>
+      <c r="P62" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q62" t="str">
-        <v>63.00</v>
-      </c>
-      <c r="R62">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R62" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S62" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>5.00</v>
+      </c>
+      <c r="T62" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U62" t="str">
+        <v>78.00</v>
+      </c>
+      <c r="V62">
+        <v>2023</v>
+      </c>
+      <c r="W62" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="63" xml:space="preserve">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3918,25 +4602,39 @@
         <v>22.00</v>
       </c>
       <c r="N63" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O63" t="str">
         <v>17.50</v>
       </c>
-      <c r="O63" t="str">
+      <c r="P63" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q63" t="str">
         <v>25.00</v>
       </c>
-      <c r="P63" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q63" t="str">
+      <c r="R63" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S63" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T63" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U63" t="str">
         <v>69.50</v>
       </c>
-      <c r="R63">
-        <v>2023</v>
-      </c>
-      <c r="S63" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="64">
+      <c r="V63">
+        <v>2023</v>
+      </c>
+      <c r="W63" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="64" xml:space="preserve">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3977,25 +4675,39 @@
         <v>20.00</v>
       </c>
       <c r="N64" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA Kejuruan</v>
       </c>
       <c r="O64" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P64" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q64" t="str">
         <v>30.00</v>
       </c>
-      <c r="P64" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q64" t="str">
-        <v>72.50</v>
-      </c>
-      <c r="R64">
-        <v>2023</v>
+      <c r="R64" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S64" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>5.00</v>
+      </c>
+      <c r="T64" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U64" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V64">
+        <v>2023</v>
+      </c>
+      <c r="W64" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="65" xml:space="preserve">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4036,25 +4748,39 @@
         <v>23.00</v>
       </c>
       <c r="N65" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O65" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P65" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q65" t="str">
         <v>30.00</v>
       </c>
-      <c r="P65" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q65" t="str">
-        <v>75.50</v>
-      </c>
-      <c r="R65">
-        <v>2023</v>
+      <c r="R65" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S65" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>5.00</v>
+      </c>
+      <c r="T65" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U65" t="str">
+        <v>98.00</v>
+      </c>
+      <c r="V65">
+        <v>2023</v>
+      </c>
+      <c r="W65" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="66" xml:space="preserve">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4095,25 +4821,39 @@
         <v>21.00</v>
       </c>
       <c r="N66" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma III/Sarjana Muda</v>
       </c>
       <c r="O66" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P66" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 130 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q66" t="str">
         <v>25.00</v>
       </c>
-      <c r="P66" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q66" t="str">
-        <v>68.50</v>
-      </c>
-      <c r="R66">
-        <v>2023</v>
+      <c r="R66" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S66" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>5.00</v>
+      </c>
+      <c r="T66" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U66" t="str">
+        <v>91.00</v>
+      </c>
+      <c r="V66">
+        <v>2023</v>
+      </c>
+      <c r="W66" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="67" xml:space="preserve">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4154,25 +4894,39 @@
         <v>22.00</v>
       </c>
       <c r="N67" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O67" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P67" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q67" t="str">
         <v>25.00</v>
       </c>
-      <c r="P67" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q67" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R67">
-        <v>2023</v>
+      <c r="R67" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S67" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>5.00</v>
+      </c>
+      <c r="T67" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U67" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V67">
+        <v>2023</v>
+      </c>
+      <c r="W67" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="68" xml:space="preserve">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4213,25 +4967,39 @@
         <v>23.00</v>
       </c>
       <c r="N68" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O68" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="P68" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 20 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q68" t="str">
         <v>30.00</v>
       </c>
-      <c r="P68" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q68" t="str">
-        <v>68.00</v>
-      </c>
-      <c r="R68">
-        <v>2023</v>
+      <c r="R68" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S68" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>5.00</v>
+      </c>
+      <c r="T68" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U68" t="str">
+        <v>83.00</v>
+      </c>
+      <c r="V68">
+        <v>2023</v>
+      </c>
+      <c r="W68" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="69" xml:space="preserve">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4272,25 +5040,39 @@
         <v>23.00</v>
       </c>
       <c r="N69" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O69" t="str">
         <v>25.00</v>
       </c>
-      <c r="P69" t="str">
-        <v>5.00</v>
+      <c r="P69" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q69" t="str">
-        <v>63.00</v>
-      </c>
-      <c r="R69">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R69" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S69" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>5.00</v>
+      </c>
+      <c r="T69" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U69" t="str">
+        <v>78.00</v>
+      </c>
+      <c r="V69">
+        <v>2023</v>
+      </c>
+      <c r="W69" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="70" xml:space="preserve">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4331,25 +5113,39 @@
         <v>22.00</v>
       </c>
       <c r="N70" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O70" t="str">
         <v>40.00</v>
       </c>
-      <c r="O70" t="str">
+      <c r="P70" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q70" t="str">
         <v>30.00</v>
       </c>
-      <c r="P70" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q70" t="str">
+      <c r="R70" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
+      </c>
+      <c r="S70" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T70" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U70" t="str">
         <v>97.00</v>
       </c>
-      <c r="R70">
-        <v>2023</v>
-      </c>
-      <c r="S70" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="71">
+      <c r="V70">
+        <v>2023</v>
+      </c>
+      <c r="W70" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="71" xml:space="preserve">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4387,25 +5183,39 @@
         <v>20.00</v>
       </c>
       <c r="N71" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA</v>
       </c>
       <c r="O71" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P71" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q71" t="str">
         <v>25.00</v>
       </c>
-      <c r="P71" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q71" t="str">
-        <v>67.50</v>
-      </c>
-      <c r="R71">
-        <v>2023</v>
+      <c r="R71" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S71" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>5.00</v>
+      </c>
+      <c r="T71" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U71" t="str">
+        <v>90.00</v>
+      </c>
+      <c r="V71">
+        <v>2023</v>
+      </c>
+      <c r="W71" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="72" xml:space="preserve">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4446,22 +5256,36 @@
         <v>21.00</v>
       </c>
       <c r="N72" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O72" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="P72" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q72" t="str">
         <v>30.00</v>
       </c>
-      <c r="P72" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q72" t="str">
-        <v>66.00</v>
-      </c>
-      <c r="R72">
-        <v>2023</v>
+      <c r="R72" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S72" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T72" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U72" t="str">
+        <v>81.00</v>
+      </c>
+      <c r="V72">
+        <v>2023</v>
+      </c>
+      <c r="W72" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="73">
@@ -4501,29 +5325,8 @@
       <c r="L73" t="str">
         <v>PNS</v>
       </c>
-      <c r="M73" t="str">
-        <v>22.00</v>
-      </c>
-      <c r="N73" t="str">
-        <v>17.50</v>
-      </c>
-      <c r="O73" t="str">
-        <v>25.00</v>
-      </c>
-      <c r="P73" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q73" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R73">
-        <v>2023</v>
-      </c>
-      <c r="S73" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="74">
+    </row>
+    <row r="74" xml:space="preserve">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4564,25 +5367,39 @@
         <v>21.00</v>
       </c>
       <c r="N74" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma III/Sarjana Muda</v>
       </c>
       <c r="O74" t="str">
         <v>25.00</v>
       </c>
-      <c r="P74" t="str">
-        <v>5.00</v>
+      <c r="P74" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q74" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="R74" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S74" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T74" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U74" t="str">
         <v>76.00</v>
       </c>
-      <c r="R74">
-        <v>2023</v>
-      </c>
-      <c r="S74" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="75">
+      <c r="V74">
+        <v>2023</v>
+      </c>
+      <c r="W74" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="75" xml:space="preserve">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4623,25 +5440,39 @@
         <v>20.00</v>
       </c>
       <c r="N75" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O75" t="str">
         <v>25.00</v>
       </c>
-      <c r="P75" t="str">
-        <v>5.00</v>
+      <c r="P75" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q75" t="str">
-        <v>60.00</v>
-      </c>
-      <c r="R75">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R75" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S75" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>5.00</v>
+      </c>
+      <c r="T75" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U75" t="str">
+        <v>75.00</v>
+      </c>
+      <c r="V75">
+        <v>2023</v>
+      </c>
+      <c r="W75" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="76" xml:space="preserve">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4682,22 +5513,36 @@
         <v>20.00</v>
       </c>
       <c r="N76" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O76" t="str">
         <v>25.00</v>
       </c>
-      <c r="P76" t="str">
-        <v>5.00</v>
+      <c r="P76" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q76" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="R76" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S76" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T76" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U76" t="str">
         <v>75.00</v>
       </c>
-      <c r="R76">
-        <v>2023</v>
-      </c>
-      <c r="S76" t="str">
-        <v>8-March-2024</v>
+      <c r="V76">
+        <v>2023</v>
+      </c>
+      <c r="W76" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="77">
@@ -4734,29 +5579,8 @@
       <c r="L77" t="str">
         <v>PNS</v>
       </c>
-      <c r="M77" t="str">
-        <v>22.00</v>
-      </c>
-      <c r="N77" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="O77" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="P77" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q77" t="str">
-        <v>27.00</v>
-      </c>
-      <c r="R77">
-        <v>2023</v>
-      </c>
-      <c r="S77" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="78">
+    </row>
+    <row r="78" xml:space="preserve">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4797,25 +5621,39 @@
         <v>23.00</v>
       </c>
       <c r="N78" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O78" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P78" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q78" t="str">
         <v>30.00</v>
       </c>
-      <c r="P78" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q78" t="str">
-        <v>83.00</v>
-      </c>
-      <c r="R78">
-        <v>2023</v>
+      <c r="R78" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S78" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>5.00</v>
+      </c>
+      <c r="T78" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U78" t="str">
+        <v>98.00</v>
+      </c>
+      <c r="V78">
+        <v>2023</v>
+      </c>
+      <c r="W78" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="79" xml:space="preserve">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4856,25 +5694,39 @@
         <v>20.00</v>
       </c>
       <c r="N79" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O79" t="str">
         <v>25.00</v>
       </c>
-      <c r="P79" t="str">
-        <v>5.00</v>
+      <c r="P79" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q79" t="str">
-        <v>60.00</v>
-      </c>
-      <c r="R79">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R79" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S79" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>5.00</v>
+      </c>
+      <c r="T79" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U79" t="str">
+        <v>75.00</v>
+      </c>
+      <c r="V79">
+        <v>2023</v>
+      </c>
+      <c r="W79" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="80" xml:space="preserve">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4915,25 +5767,39 @@
         <v>22.00</v>
       </c>
       <c r="N80" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma IV</v>
       </c>
       <c r="O80" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P80" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q80" t="str">
         <v>25.00</v>
       </c>
-      <c r="P80" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q80" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R80">
-        <v>2023</v>
+      <c r="R80" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S80" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>5.00</v>
+      </c>
+      <c r="T80" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U80" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V80">
+        <v>2023</v>
+      </c>
+      <c r="W80" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="81" xml:space="preserve">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4974,25 +5840,39 @@
         <v>22.00</v>
       </c>
       <c r="N81" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O81" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P81" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q81" t="str">
         <v>25.00</v>
       </c>
-      <c r="P81" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q81" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R81">
-        <v>2023</v>
+      <c r="R81" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S81" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>5.00</v>
+      </c>
+      <c r="T81" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U81" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V81">
+        <v>2023</v>
+      </c>
+      <c r="W81" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="82" xml:space="preserve">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5033,25 +5913,39 @@
         <v>22.00</v>
       </c>
       <c r="N82" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O82" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P82" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q82" t="str">
         <v>25.00</v>
       </c>
-      <c r="P82" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q82" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R82">
-        <v>2023</v>
+      <c r="R82" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S82" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>5.00</v>
+      </c>
+      <c r="T82" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U82" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V82">
+        <v>2023</v>
+      </c>
+      <c r="W82" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="83" xml:space="preserve">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5092,25 +5986,39 @@
         <v>20.00</v>
       </c>
       <c r="N83" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O83" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="P83" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q83" t="str">
         <v>30.00</v>
       </c>
-      <c r="P83" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q83" t="str">
-        <v>65.00</v>
-      </c>
-      <c r="R83">
-        <v>2023</v>
+      <c r="R83" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S83" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="84">
+        <v>5.00</v>
+      </c>
+      <c r="T83" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U83" t="str">
+        <v>80.00</v>
+      </c>
+      <c r="V83">
+        <v>2023</v>
+      </c>
+      <c r="W83" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="84" xml:space="preserve">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5151,25 +6059,39 @@
         <v>22.00</v>
       </c>
       <c r="N84" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O84" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P84" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q84" t="str">
         <v>25.00</v>
       </c>
-      <c r="P84" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q84" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R84">
-        <v>2023</v>
+      <c r="R84" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S84" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>5.00</v>
+      </c>
+      <c r="T84" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U84" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V84">
+        <v>2023</v>
+      </c>
+      <c r="W84" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="85" xml:space="preserve">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5210,25 +6132,39 @@
         <v>21.00</v>
       </c>
       <c r="N85" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah Diploma III/Sarjana Muda</v>
       </c>
       <c r="O85" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P85" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 54 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q85" t="str">
         <v>25.00</v>
       </c>
-      <c r="P85" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q85" t="str">
-        <v>68.50</v>
-      </c>
-      <c r="R85">
-        <v>2023</v>
+      <c r="R85" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S85" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="86">
+        <v>5.00</v>
+      </c>
+      <c r="T85" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U85" t="str">
+        <v>91.00</v>
+      </c>
+      <c r="V85">
+        <v>2023</v>
+      </c>
+      <c r="W85" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="86" xml:space="preserve">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5269,25 +6205,39 @@
         <v>22.00</v>
       </c>
       <c r="N86" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O86" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P86" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q86" t="str">
         <v>30.00</v>
       </c>
-      <c r="P86" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q86" t="str">
-        <v>74.50</v>
-      </c>
-      <c r="R86">
-        <v>2023</v>
+      <c r="R86" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S86" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>5.00</v>
+      </c>
+      <c r="T86" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U86" t="str">
+        <v>97.00</v>
+      </c>
+      <c r="V86">
+        <v>2023</v>
+      </c>
+      <c r="W86" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="87" xml:space="preserve">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5328,25 +6278,39 @@
         <v>22.00</v>
       </c>
       <c r="N87" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O87" t="str">
         <v>17.50</v>
       </c>
-      <c r="O87" t="str">
+      <c r="P87" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda belum melaksanakan Diklat Teknis tahun 2023_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q87" t="str">
         <v>25.00</v>
       </c>
-      <c r="P87" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q87" t="str">
+      <c r="R87" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S87" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T87" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U87" t="str">
         <v>69.50</v>
       </c>
-      <c r="R87">
-        <v>2023</v>
-      </c>
-      <c r="S87" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="88">
+      <c r="V87">
+        <v>2023</v>
+      </c>
+      <c r="W87" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="88" xml:space="preserve">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5387,25 +6351,39 @@
         <v>23.00</v>
       </c>
       <c r="N88" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O88" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P88" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q88" t="str">
         <v>25.00</v>
       </c>
-      <c r="P88" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q88" t="str">
-        <v>70.50</v>
-      </c>
-      <c r="R88">
-        <v>2023</v>
+      <c r="R88" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S88" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>5.00</v>
+      </c>
+      <c r="T88" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U88" t="str">
+        <v>93.00</v>
+      </c>
+      <c r="V88">
+        <v>2023</v>
+      </c>
+      <c r="W88" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="89" xml:space="preserve">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5446,25 +6424,39 @@
         <v>22.00</v>
       </c>
       <c r="N89" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O89" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P89" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q89" t="str">
         <v>25.00</v>
       </c>
-      <c r="P89" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q89" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R89">
-        <v>2023</v>
+      <c r="R89" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S89" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>5.00</v>
+      </c>
+      <c r="T89" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U89" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V89">
+        <v>2023</v>
+      </c>
+      <c r="W89" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="90" xml:space="preserve">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5502,25 +6494,39 @@
         <v>20.00</v>
       </c>
       <c r="N90" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA</v>
       </c>
       <c r="O90" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P90" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q90" t="str">
         <v>25.00</v>
       </c>
-      <c r="P90" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q90" t="str">
-        <v>67.50</v>
-      </c>
-      <c r="R90">
-        <v>2023</v>
+      <c r="R90" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S90" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="91">
+        <v>5.00</v>
+      </c>
+      <c r="T90" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U90" t="str">
+        <v>90.00</v>
+      </c>
+      <c r="V90">
+        <v>2023</v>
+      </c>
+      <c r="W90" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="91" xml:space="preserve">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5561,25 +6567,39 @@
         <v>22.00</v>
       </c>
       <c r="N91" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O91" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P91" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q91" t="str">
         <v>25.00</v>
       </c>
-      <c r="P91" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q91" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R91">
-        <v>2023</v>
+      <c r="R91" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S91" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>5.00</v>
+      </c>
+      <c r="T91" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U91" t="str">
+        <v>92.00</v>
+      </c>
+      <c r="V91">
+        <v>2023</v>
+      </c>
+      <c r="W91" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="92" xml:space="preserve">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5620,22 +6640,36 @@
         <v>20.00</v>
       </c>
       <c r="N92" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O92" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P92" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q92" t="str">
         <v>30.00</v>
       </c>
-      <c r="P92" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q92" t="str">
-        <v>80.00</v>
-      </c>
-      <c r="R92">
-        <v>2023</v>
+      <c r="R92" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S92" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T92" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U92" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V92">
+        <v>2023</v>
+      </c>
+      <c r="W92" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="93">
@@ -5675,29 +6709,8 @@
       <c r="L93" t="str">
         <v>PNS</v>
       </c>
-      <c r="M93" t="str">
-        <v>22.00</v>
-      </c>
-      <c r="N93" t="str">
-        <v>17.50</v>
-      </c>
-      <c r="O93" t="str">
-        <v>25.00</v>
-      </c>
-      <c r="P93" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q93" t="str">
-        <v>69.50</v>
-      </c>
-      <c r="R93">
-        <v>2023</v>
-      </c>
-      <c r="S93" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="94">
+    </row>
+    <row r="94" xml:space="preserve">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5735,22 +6748,36 @@
         <v>20.00</v>
       </c>
       <c r="N94" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA</v>
       </c>
       <c r="O94" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P94" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q94" t="str">
         <v>30.00</v>
       </c>
-      <c r="P94" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q94" t="str">
-        <v>72.50</v>
-      </c>
-      <c r="R94">
-        <v>2023</v>
+      <c r="R94" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S94" t="str">
-        <v>8-March-2024</v>
+        <v>5.00</v>
+      </c>
+      <c r="T94" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U94" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V94">
+        <v>2023</v>
+      </c>
+      <c r="W94" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
     <row r="95">
@@ -5790,27 +6817,6 @@
       <c r="L95" t="str">
         <v>PNS</v>
       </c>
-      <c r="M95" t="str">
-        <v>22.00</v>
-      </c>
-      <c r="N95" t="str">
-        <v>40.00</v>
-      </c>
-      <c r="O95" t="str">
-        <v>30.00</v>
-      </c>
-      <c r="P95" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q95" t="str">
-        <v>97.00</v>
-      </c>
-      <c r="R95">
-        <v>2023</v>
-      </c>
-      <c r="S95" t="str">
-        <v>8-March-2024</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -5850,7 +6856,7 @@
         <v>PPPK</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" xml:space="preserve">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5891,25 +6897,39 @@
         <v>22.00</v>
       </c>
       <c r="N97" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O97" t="str">
         <v>22.50</v>
       </c>
-      <c r="O97" t="str">
+      <c r="P97" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 102 Jam_x000d_
+Anda belum sama sekali melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q97" t="str">
         <v>25.00</v>
       </c>
-      <c r="P97" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q97" t="str">
+      <c r="R97" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S97" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T97" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U97" t="str">
         <v>74.50</v>
       </c>
-      <c r="R97">
-        <v>2023</v>
-      </c>
-      <c r="S97" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="98">
+      <c r="V97">
+        <v>2023</v>
+      </c>
+      <c r="W97" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="98" xml:space="preserve">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5947,25 +6967,39 @@
         <v>20.00</v>
       </c>
       <c r="N98" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA</v>
       </c>
       <c r="O98" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P98" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q98" t="str">
         <v>25.00</v>
       </c>
-      <c r="P98" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q98" t="str">
-        <v>67.50</v>
-      </c>
-      <c r="R98">
-        <v>2023</v>
+      <c r="R98" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S98" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="99">
+        <v>5.00</v>
+      </c>
+      <c r="T98" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U98" t="str">
+        <v>90.00</v>
+      </c>
+      <c r="V98">
+        <v>2023</v>
+      </c>
+      <c r="W98" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="99" xml:space="preserve">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6003,25 +7037,39 @@
         <v>20.00</v>
       </c>
       <c r="N99" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah SLTA</v>
       </c>
       <c r="O99" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P99" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q99" t="str">
         <v>30.00</v>
       </c>
-      <c r="P99" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q99" t="str">
-        <v>72.50</v>
-      </c>
-      <c r="R99">
-        <v>2023</v>
+      <c r="R99" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S99" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>5.00</v>
+      </c>
+      <c r="T99" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U99" t="str">
+        <v>95.00</v>
+      </c>
+      <c r="V99">
+        <v>2023</v>
+      </c>
+      <c r="W99" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="100" xml:space="preserve">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6062,25 +7110,39 @@
         <v>20.00</v>
       </c>
       <c r="N100" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O100" t="str">
+        <v>25.00</v>
+      </c>
+      <c r="P100" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q100" t="str">
         <v>30.00</v>
       </c>
-      <c r="P100" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q100" t="str">
-        <v>65.00</v>
-      </c>
-      <c r="R100">
-        <v>2023</v>
+      <c r="R100" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S100" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>5.00</v>
+      </c>
+      <c r="T100" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U100" t="str">
+        <v>80.00</v>
+      </c>
+      <c r="V100">
+        <v>2023</v>
+      </c>
+      <c r="W100" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="101" xml:space="preserve">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6121,25 +7183,39 @@
         <v>20.00</v>
       </c>
       <c r="N101" t="str">
-        <v>10.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O101" t="str">
         <v>25.00</v>
       </c>
-      <c r="P101" t="str">
-        <v>5.00</v>
+      <c r="P101" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
       </c>
       <c r="Q101" t="str">
-        <v>60.00</v>
-      </c>
-      <c r="R101">
-        <v>2023</v>
+        <v>25.00</v>
+      </c>
+      <c r="R101" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
       </c>
       <c r="S101" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="102">
+        <v>5.00</v>
+      </c>
+      <c r="T101" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U101" t="str">
+        <v>75.00</v>
+      </c>
+      <c r="V101">
+        <v>2023</v>
+      </c>
+      <c r="W101" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="102" xml:space="preserve">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6165,10 +7241,10 @@
         <v>MAGISTER SOSIOLOGI</v>
       </c>
       <c r="I102" t="str">
-        <v>III/c</v>
+        <v>III/d</v>
       </c>
       <c r="J102" t="str">
-        <v>Penata</v>
+        <v>Penata Tingkat I</v>
       </c>
       <c r="K102" t="str">
         <v>Analis Sumber Daya Manusia Aparatur Ahli Muda (III/c)</v>
@@ -6180,25 +7256,39 @@
         <v>23.00</v>
       </c>
       <c r="N102" t="str">
-        <v>25.00</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-2</v>
       </c>
       <c r="O102" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P102" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q102" t="str">
         <v>30.00</v>
       </c>
-      <c r="P102" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q102" t="str">
-        <v>83.00</v>
-      </c>
-      <c r="R102">
-        <v>2023</v>
+      <c r="R102" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S102" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="103">
+        <v>5.00</v>
+      </c>
+      <c r="T102" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U102" t="str">
+        <v>98.00</v>
+      </c>
+      <c r="V102">
+        <v>2023</v>
+      </c>
+      <c r="W102" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="103" xml:space="preserve">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6239,25 +7329,39 @@
         <v>22.00</v>
       </c>
       <c r="N103" t="str">
-        <v>17.50</v>
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
       </c>
       <c r="O103" t="str">
+        <v>40.00</v>
+      </c>
+      <c r="P103" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 26 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q103" t="str">
         <v>30.00</v>
       </c>
-      <c r="P103" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q103" t="str">
-        <v>74.50</v>
-      </c>
-      <c r="R103">
-        <v>2023</v>
+      <c r="R103" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'SANGAT BAIK'</v>
       </c>
       <c r="S103" t="str">
-        <v>8-March-2024</v>
-      </c>
-    </row>
-    <row r="104">
+        <v>5.00</v>
+      </c>
+      <c r="T103" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U103" t="str">
+        <v>97.00</v>
+      </c>
+      <c r="V103">
+        <v>2023</v>
+      </c>
+      <c r="W103" t="str">
+        <v>2024-03-15T03:03:44Z</v>
+      </c>
+    </row>
+    <row r="104" xml:space="preserve">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6298,27 +7402,41 @@
         <v>22.00</v>
       </c>
       <c r="N104" t="str">
+        <v>Sesuai, kualifikasi pendidikan anda saat ini adalah S-1/Sarjana</v>
+      </c>
+      <c r="O104" t="str">
         <v>40.00</v>
       </c>
-      <c r="O104" t="str">
+      <c r="P104" t="str" xml:space="preserve">
+        <v xml:space="preserve">_x000d_
+Anda sudah melaksanakan Diklat Teknis tahun 2023 Selama : 52 Jam_x000d_
+Anda sudah melaksanakan Diklat Pendukung/Seminar/Workshop/Sejenisnya selama 2 tahun terakhir</v>
+      </c>
+      <c r="Q104" t="str">
         <v>25.00</v>
       </c>
-      <c r="P104" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="Q104" t="str">
+      <c r="R104" t="str">
+        <v>Nilai Prestasi Kerja Tahun 2023 adalah, 'BAIK'</v>
+      </c>
+      <c r="S104" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="T104" t="str">
+        <v>Dalam 1 Tahun Terkahir anda tidak dijatuhi hukuman disiplin dan/atau tidak terdapat Riwayat Hukuman Disiplin</v>
+      </c>
+      <c r="U104" t="str">
         <v>92.00</v>
       </c>
-      <c r="R104">
-        <v>2023</v>
-      </c>
-      <c r="S104" t="str">
-        <v>8-March-2024</v>
+      <c r="V104">
+        <v>2023</v>
+      </c>
+      <c r="W104" t="str">
+        <v>2024-03-15T03:03:44Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S104"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W104"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>